<commit_message>
Cleaned up / Added Research Plan
</commit_message>
<xml_diff>
--- a/Foil_Activation/FoilInfoUPdated.xlsx
+++ b/Foil_Activation/FoilInfoUPdated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickq\Documents\AFIT_Masters\NENG612\Foil_Activation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BD372D7E-8EE8-4F43-83BD-893FCC9706A9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{77675AA2-D1DD-4555-8F14-DAF7DBA09CBD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" firstSheet="6" activeTab="7" xr2:uid="{A54BA526-0B45-47AA-953D-39C722521EAC}"/>
   </bookViews>
@@ -22,6 +22,38 @@
     <sheet name="Flux Spectra" sheetId="7" r:id="rId7"/>
     <sheet name="Consolidated Data" sheetId="8" r:id="rId8"/>
   </sheets>
+  <definedNames>
+    <definedName name="solver_adj" localSheetId="7" hidden="1">'Consolidated Data'!$R$4:$R$7</definedName>
+    <definedName name="solver_cvg" localSheetId="7" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="7" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="7" hidden="1">'Consolidated Data'!$N$5</definedName>
+    <definedName name="solver_mip" localSheetId="7" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="7" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="7" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="7" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="7" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="7" hidden="1">'Consolidated Data'!$S$7</definedName>
+    <definedName name="solver_pre" localSheetId="7" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="7" hidden="1">3</definedName>
+    <definedName name="solver_rhs1" localSheetId="7" hidden="1">0.01</definedName>
+    <definedName name="solver_rlx" localSheetId="7" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="7" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="7" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="7" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="7" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="7" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="7" hidden="1">3</definedName>
+    <definedName name="solver_val" localSheetId="7" hidden="1">10000</definedName>
+    <definedName name="solver_ver" localSheetId="7" hidden="1">3</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="178">
   <si>
     <t>Foil</t>
   </si>
@@ -506,15 +538,76 @@
   </si>
   <si>
     <t>Timing of foils to HPGe is extremely important. Escpecially for the HPGE</t>
+  </si>
+  <si>
+    <t>Density [g/cc]</t>
+  </si>
+  <si>
+    <t>Mn</t>
+  </si>
+  <si>
+    <t>Mass Per</t>
+  </si>
+  <si>
+    <t>Note: W and In from ShieldWerx. Au and Mn from supply room foils</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volume </t>
+  </si>
+  <si>
+    <t>Per foil -cc</t>
+  </si>
+  <si>
+    <t>Foil -g</t>
+  </si>
+  <si>
+    <t>Approximate Efficiency</t>
+  </si>
+  <si>
+    <t>Counts/s</t>
+  </si>
+  <si>
+    <t>10,000 count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time [hr]to </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Counts </t>
+  </si>
+  <si>
+    <t>in Time</t>
+  </si>
+  <si>
+    <t>Approximate</t>
+  </si>
+  <si>
+    <t>20 min</t>
+  </si>
+  <si>
+    <t>Count Plan</t>
+  </si>
+  <si>
+    <t>3 hours</t>
+  </si>
+  <si>
+    <t>3 Hrs</t>
+  </si>
+  <si>
+    <t>Count Mn and In for 10,000 Counts --&gt;3-5 Hrs</t>
+  </si>
+  <si>
+    <t>Count W and Au for 1 day after Mn and In</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000E+00"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -525,15 +618,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -541,11 +640,128 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -554,6 +770,35 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -871,7 +1116,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -979,6 +1224,10 @@
       </c>
       <c r="F4">
         <v>0.63500000000000001</v>
+      </c>
+      <c r="I4">
+        <f>I3*2</f>
+        <v>1.27</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -3347,7 +3596,7 @@
         <v>0</v>
       </c>
       <c r="M4" s="1">
-        <f>K4*EXP(-E4*24*60*60)</f>
+        <f t="shared" ref="M4:M20" si="2">K4*EXP(-E4*24*60*60)</f>
         <v>0</v>
       </c>
       <c r="O4" s="2"/>
@@ -3369,15 +3618,15 @@
         <v>6678720</v>
       </c>
       <c r="E5" s="5">
-        <f t="shared" ref="E5:E20" si="2">LN(2)/D5</f>
+        <f t="shared" ref="E5:E20" si="3">LN(2)/D5</f>
         <v>1.0378443482582669E-7</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" ref="F5:F19" si="3">4*D5/3600</f>
+        <f t="shared" ref="F5:F19" si="4">4*D5/3600</f>
         <v>7420.8</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" ref="G5:G20" si="4">F5/24</f>
+        <f t="shared" ref="G5:G20" si="5">F5/24</f>
         <v>309.2</v>
       </c>
       <c r="H5" s="2">
@@ -3396,11 +3645,11 @@
         <v>0.24318624125174951</v>
       </c>
       <c r="L5" s="1">
-        <f t="shared" ref="L5:L20" si="5">K5*EXP(-E5*60*60)</f>
+        <f t="shared" ref="L5:L20" si="6">K5*EXP(-E5*60*60)</f>
         <v>0.24309539801563071</v>
       </c>
       <c r="M5" s="1">
-        <f>K5*EXP(-E5*24*60*60)</f>
+        <f t="shared" si="2"/>
         <v>0.2410153440020745</v>
       </c>
       <c r="O5" s="2"/>
@@ -3421,15 +3670,15 @@
         <v>567.48</v>
       </c>
       <c r="E6" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.2214477700710955E-3</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.63053333333333339</v>
       </c>
       <c r="G6" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.6272222222222225E-2</v>
       </c>
       <c r="H6" s="2">
@@ -3448,11 +3697,11 @@
         <v>3.693397778822545E-2</v>
       </c>
       <c r="L6" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.5471699724364706E-4</v>
       </c>
       <c r="M6" s="1">
-        <f>K6*EXP(-E6*24*60*60)</f>
+        <f t="shared" si="2"/>
         <v>5.4323606694259364E-48</v>
       </c>
       <c r="O6" s="2"/>
@@ -3473,15 +3722,15 @@
         <v>53989.2</v>
       </c>
       <c r="E7" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.2838626624583163E-5</v>
       </c>
       <c r="F7" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>59.988</v>
       </c>
       <c r="G7" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.4994999999999998</v>
       </c>
       <c r="H7" s="2">
@@ -3500,11 +3749,11 @@
         <v>9.7068639852089991E-3</v>
       </c>
       <c r="L7" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9.268431900546905E-3</v>
       </c>
       <c r="M7" s="1">
-        <f>K7*EXP(-E7*24*60*60)</f>
+        <f t="shared" si="2"/>
         <v>3.2013606489719108E-3</v>
       </c>
       <c r="O7" s="2"/>
@@ -3526,15 +3775,15 @@
         <v>532820.16</v>
       </c>
       <c r="E8" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3009026921202555E-6</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>592.02240000000006</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>24.667600000000004</v>
       </c>
       <c r="H8" s="2">
@@ -3552,11 +3801,11 @@
         <v>2.0249780300813626E-2</v>
       </c>
       <c r="L8" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.0155167244674792E-2</v>
       </c>
       <c r="M8" s="1">
-        <f>K8*EXP(-E8*24*60*60)</f>
+        <f t="shared" si="2"/>
         <v>1.8096995889699482E-2</v>
       </c>
       <c r="O8" s="2"/>
@@ -3578,15 +3827,15 @@
         <v>232770.24</v>
       </c>
       <c r="E9" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.9778170120026741E-6</v>
       </c>
       <c r="F9" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>258.6336</v>
       </c>
       <c r="G9" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>10.776400000000001</v>
       </c>
       <c r="H9" s="2">
@@ -3605,11 +3854,11 @@
         <v>152.4914110262271</v>
       </c>
       <c r="L9" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>150.86541259985421</v>
       </c>
       <c r="M9" s="1">
-        <f>K9*EXP(-E9*24*60*60)</f>
+        <f t="shared" si="2"/>
         <v>117.89859416188695</v>
       </c>
       <c r="O9" s="2"/>
@@ -3630,19 +3879,19 @@
         <v>9284.0399999999991</v>
       </c>
       <c r="E10" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.4660081231871619E-5</v>
       </c>
       <c r="F10" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10.315599999999998</v>
       </c>
       <c r="G10" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.42981666666666657</v>
       </c>
       <c r="H10" s="2">
-        <f>PI()*0.635^2*0.0127</f>
+        <f t="shared" ref="H10:H20" si="7">PI()*0.635^2*0.0127</f>
         <v>1.6087962461345549E-2</v>
       </c>
       <c r="I10" s="2">
@@ -3657,11 +3906,11 @@
         <v>117.84331953170232</v>
       </c>
       <c r="L10" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>90.069324779102146</v>
       </c>
       <c r="M10" s="1">
-        <f>K10*EXP(-E10*24*60*60)</f>
+        <f t="shared" si="2"/>
         <v>0.18613648633715099</v>
       </c>
       <c r="O10" s="2"/>
@@ -3682,19 +3931,19 @@
         <v>9913536</v>
       </c>
       <c r="E11" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.9919268014959077E-8</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11015.04</v>
       </c>
       <c r="G11" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>458.96000000000004</v>
       </c>
       <c r="H11" s="2">
-        <f>PI()*0.635^2*0.0127</f>
+        <f t="shared" si="7"/>
         <v>1.6087962461345549E-2</v>
       </c>
       <c r="I11" s="2">
@@ -3709,11 +3958,11 @@
         <v>7.7301897459404092</v>
       </c>
       <c r="L11" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7.7282442296518647</v>
       </c>
       <c r="M11" s="1">
-        <f>K11*EXP(-E11*24*60*60)</f>
+        <f t="shared" si="2"/>
         <v>7.6836322474023833</v>
       </c>
       <c r="O11" s="2"/>
@@ -3734,19 +3983,19 @@
         <v>510.59999999999997</v>
       </c>
       <c r="E12" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3575150422247264E-3</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.56733333333333325</v>
       </c>
       <c r="G12" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.3638888888888886E-2</v>
       </c>
       <c r="H12" s="2">
-        <f>PI()*0.635^2*0.0127</f>
+        <f t="shared" si="7"/>
         <v>1.6087962461345549E-2</v>
       </c>
       <c r="I12" s="2">
@@ -3761,11 +4010,11 @@
         <v>0</v>
       </c>
       <c r="L12" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M12" s="1">
-        <f>K12*EXP(-E12*24*60*60)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O12" s="2"/>
@@ -3786,19 +4035,19 @@
         <v>26974079.999999996</v>
       </c>
       <c r="E13" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.5696786713761706E-8</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>29971.199999999997</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1248.8</v>
       </c>
       <c r="H13" s="2">
-        <f>PI()*0.635^2*0.0127</f>
+        <f t="shared" si="7"/>
         <v>1.6087962461345549E-2</v>
       </c>
       <c r="I13" s="2">
@@ -3813,11 +4062,11 @@
         <v>1.5950630205204073E-3</v>
       </c>
       <c r="L13" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.5949154705660799E-3</v>
       </c>
       <c r="M13" s="1">
-        <f>K13*EXP(-E13*24*60*60)</f>
+        <f t="shared" si="2"/>
         <v>1.5915255861817922E-3</v>
       </c>
       <c r="O13" s="2"/>
@@ -3834,23 +4083,23 @@
         <v>73</v>
       </c>
       <c r="D14" s="5">
-        <f t="shared" ref="D14:D16" si="6">B14*24*3600</f>
+        <f t="shared" ref="D14:D16" si="8">B14*24*3600</f>
         <v>2393496</v>
       </c>
       <c r="E14" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.8959613074763664E-7</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2659.44</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>110.81</v>
       </c>
       <c r="H14" s="2">
-        <f>PI()*0.635^2*0.0127</f>
+        <f t="shared" si="7"/>
         <v>1.6087962461345549E-2</v>
       </c>
       <c r="I14" s="2">
@@ -3865,11 +4114,11 @@
         <v>3.2957931620216198E-4</v>
       </c>
       <c r="L14" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.292358936291069E-4</v>
       </c>
       <c r="M14" s="1">
-        <f>K14*EXP(-E14*24*60*60)</f>
+        <f t="shared" si="2"/>
         <v>3.2143518970630726E-4</v>
       </c>
       <c r="Q14" s="2"/>
@@ -3889,19 +4138,19 @@
         <v>9284.0399999999991</v>
       </c>
       <c r="E15" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.4660081231871619E-5</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10.315599999999998</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.42981666666666657</v>
       </c>
       <c r="H15" s="2">
-        <f>PI()*0.635^2*0.0127</f>
+        <f t="shared" si="7"/>
         <v>1.6087962461345549E-2</v>
       </c>
       <c r="I15" s="2">
@@ -3916,11 +4165,11 @@
         <v>4.5016026677433513E-2</v>
       </c>
       <c r="L15" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.440638929034686E-2</v>
       </c>
       <c r="M15" s="1">
-        <f>K15*EXP(-E15*24*60*60)</f>
+        <f t="shared" si="2"/>
         <v>7.1103946052222049E-5</v>
       </c>
       <c r="Q15" s="2"/>
@@ -3936,23 +4185,23 @@
         <v>73</v>
       </c>
       <c r="D16" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3844367.9999999995</v>
       </c>
       <c r="E16" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.8030198476315103E-7</v>
       </c>
       <c r="F16" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4271.5199999999995</v>
       </c>
       <c r="G16" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>177.98</v>
       </c>
       <c r="H16" s="2">
-        <f>PI()*0.635^2*0.0127</f>
+        <f t="shared" si="7"/>
         <v>1.6087962461345549E-2</v>
       </c>
       <c r="I16" s="2">
@@ -3967,11 +4216,11 @@
         <v>3.5366539900929615E-3</v>
       </c>
       <c r="L16" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.5343591383111251E-3</v>
       </c>
       <c r="M16" s="1">
-        <f>K16*EXP(-E16*24*60*60)</f>
+        <f t="shared" si="2"/>
         <v>3.481986583161607E-3</v>
       </c>
       <c r="Q16" s="2"/>
@@ -3991,19 +4240,19 @@
         <v>86400</v>
       </c>
       <c r="E17" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8.0225368120364038E-6</v>
       </c>
       <c r="F17" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>96</v>
       </c>
       <c r="G17" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="H17" s="2">
-        <f>PI()*0.635^2*0.0127</f>
+        <f t="shared" si="7"/>
         <v>1.6087962461345549E-2</v>
       </c>
       <c r="I17" s="2">
@@ -4018,11 +4267,11 @@
         <v>87.759164237945612</v>
       </c>
       <c r="L17" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>85.260831186109414</v>
       </c>
       <c r="M17" s="1">
-        <f>K17*EXP(-E17*24*60*60)</f>
+        <f t="shared" si="2"/>
         <v>43.879582118972806</v>
       </c>
       <c r="P17" t="s">
@@ -4046,19 +4295,19 @@
         <v>3257.4</v>
       </c>
       <c r="E18" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.1279154557620963E-4</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.6193333333333335</v>
       </c>
       <c r="G18" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.15080555555555555</v>
       </c>
       <c r="H18" s="2">
-        <f>PI()*0.635^2*0.0127</f>
+        <f t="shared" si="7"/>
         <v>1.6087962461345549E-2</v>
       </c>
       <c r="I18" s="2">
@@ -4073,11 +4322,11 @@
         <v>697.03524393796511</v>
       </c>
       <c r="L18" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>324.01389821529744</v>
       </c>
       <c r="M18" s="1">
-        <f>K18*EXP(-E18*24*60*60)</f>
+        <f t="shared" si="2"/>
         <v>7.2221810722352151E-6</v>
       </c>
       <c r="O18" s="2"/>
@@ -4102,19 +4351,19 @@
         <v>16149.599999999999</v>
       </c>
       <c r="E19" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.2920393109423474E-5</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>17.943999999999999</v>
       </c>
       <c r="G19" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.74766666666666659</v>
       </c>
       <c r="H19" s="2">
-        <f>PI()*0.635^2*0.0127</f>
+        <f t="shared" si="7"/>
         <v>1.6087962461345549E-2</v>
       </c>
       <c r="I19" s="2">
@@ -4129,11 +4378,11 @@
         <v>0.63186515710084057</v>
       </c>
       <c r="L19" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.54140228470784069</v>
       </c>
       <c r="M19" s="1">
-        <f>K19*EXP(-E19*24*60*60)</f>
+        <f t="shared" si="2"/>
         <v>1.5492469198719204E-2</v>
       </c>
       <c r="P19" s="2"/>
@@ -4154,19 +4403,19 @@
         <v>166344192</v>
       </c>
       <c r="E20" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.166945489506152E-9</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" ref="F20" si="7">4*D20/3600</f>
+        <f t="shared" ref="F20" si="9">4*D20/3600</f>
         <v>184826.88</v>
       </c>
       <c r="G20" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7701.12</v>
       </c>
       <c r="H20" s="2">
-        <f>PI()*0.635^2*0.0127</f>
+        <f t="shared" si="7"/>
         <v>1.6087962461345549E-2</v>
       </c>
       <c r="I20" s="2">
@@ -4181,11 +4430,11 @@
         <v>0.10872475570693864</v>
       </c>
       <c r="L20" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.10872312473870234</v>
       </c>
       <c r="M20" s="1">
-        <f>K20*EXP(-E20*24*60*60)</f>
+        <f t="shared" si="2"/>
         <v>0.10868561922113447</v>
       </c>
     </row>
@@ -5638,10 +5887,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D072BB63-4EA1-465F-A281-6491F24B98B3}">
-  <dimension ref="A1:R23"/>
+  <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5654,18 +5903,29 @@
     <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.21875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.6640625" customWidth="1"/>
+    <col min="13" max="13" width="11.44140625" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" customWidth="1"/>
+    <col min="15" max="15" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>14</v>
       </c>
       <c r="I1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="M1" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>110</v>
       </c>
@@ -5690,17 +5950,35 @@
       <c r="J2" t="s">
         <v>134</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="21" t="s">
         <v>135</v>
       </c>
       <c r="L2" t="s">
         <v>149</v>
       </c>
       <c r="M2" t="s">
+        <v>166</v>
+      </c>
+      <c r="N2" t="s">
+        <v>168</v>
+      </c>
+      <c r="O2" t="s">
+        <v>169</v>
+      </c>
+      <c r="P2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Q2" t="s">
+        <v>166</v>
+      </c>
+      <c r="R2" t="s">
+        <v>168</v>
+      </c>
+      <c r="S2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -5731,17 +6009,35 @@
       <c r="J3" t="s">
         <v>54</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="21" t="s">
         <v>54</v>
       </c>
       <c r="L3" t="s">
-        <v>150</v>
+        <v>172</v>
       </c>
       <c r="M3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+      <c r="N3" t="s">
+        <v>167</v>
+      </c>
+      <c r="O3" t="s">
+        <v>170</v>
+      </c>
+      <c r="P3" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>175</v>
+      </c>
+      <c r="R3" t="s">
+        <v>167</v>
+      </c>
+      <c r="S3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -5768,32 +6064,52 @@
         <v>4</v>
       </c>
       <c r="H4" s="2">
-        <f>PI()*0.635^2*0.0127</f>
-        <v>1.6087962461345549E-2</v>
+        <f>PI()*0.635^2*0.0127*2</f>
+        <v>3.2175924922691099E-2</v>
       </c>
       <c r="I4" s="2">
         <v>5.4651199999999997E-4</v>
       </c>
       <c r="J4" s="1">
         <f>I4*$B$10*H4</f>
-        <v>88.45018127918928</v>
-      </c>
-      <c r="K4" s="1">
+        <v>176.90036255837856</v>
+      </c>
+      <c r="K4" s="26">
         <f>J4*(1-EXP(-E4*$B$12))</f>
-        <v>87.759164237945612</v>
+        <v>175.51832847589122</v>
       </c>
       <c r="L4" s="1">
-        <f>K4*EXP(-E4*60*60)</f>
-        <v>85.260831186109414</v>
+        <f>K4*EXP(-E4*60*60/3)</f>
+        <v>173.83671325389454</v>
       </c>
       <c r="M4" s="1">
-        <f>K4*EXP(-E4*24*60*60)</f>
-        <v>43.879582118972806</v>
-      </c>
-      <c r="O4" s="2"/>
-      <c r="Q4" s="2"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+        <f>L4*$M$10</f>
+        <v>1.3833486102602857</v>
+      </c>
+      <c r="N4">
+        <v>8.8781126646487571</v>
+      </c>
+      <c r="O4" s="5">
+        <f t="shared" ref="O4:O6" si="0">M4*N4*3600*(1-EXP(-N4*3600*E4))</f>
+        <v>10000.00029617375</v>
+      </c>
+      <c r="P4" s="1">
+        <f>K4*EXP(-E4*60*60*3)</f>
+        <v>160.95101686891783</v>
+      </c>
+      <c r="Q4" s="1">
+        <f>P4*$M$10</f>
+        <v>1.2808074965177652</v>
+      </c>
+      <c r="R4">
+        <v>9.250412226487116</v>
+      </c>
+      <c r="S4" s="5">
+        <f>Q4*R4*3600*(1-EXP(-R4*3600*E4))</f>
+        <v>9999.9999979187505</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -5821,32 +6137,52 @@
         <v>0.15080555555555555</v>
       </c>
       <c r="H5" s="2">
-        <f>PI()*0.635^2*0.0127</f>
-        <v>1.6087962461345549E-2</v>
+        <f>PI()*0.635^2*0.0127*2</f>
+        <v>3.2175924922691099E-2</v>
       </c>
       <c r="I5" s="2">
         <v>4.3068100000000003E-3</v>
       </c>
       <c r="J5" s="1">
         <f>I5*$B$10*H5</f>
-        <v>697.03524393796511</v>
-      </c>
-      <c r="K5" s="1">
+        <v>1394.0704878759302</v>
+      </c>
+      <c r="K5" s="26">
         <f>J5*(1-EXP(-E5*$B$12))</f>
-        <v>697.03524393796511</v>
+        <v>1394.0704878759302</v>
       </c>
       <c r="L5" s="1">
-        <f>K5*EXP(-E5*60*60)</f>
-        <v>324.01389821529744</v>
+        <f t="shared" ref="L5:L7" si="1">K5*EXP(-E5*60*60/3)</f>
+        <v>1079.9103425787075</v>
       </c>
       <c r="M5" s="1">
-        <f>K5*EXP(-E5*24*60*60)</f>
-        <v>7.2221810722352151E-6</v>
-      </c>
-      <c r="O5" s="2"/>
-      <c r="Q5" s="2"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+        <f t="shared" ref="M5:M7" si="2">L5*$M$10</f>
+        <v>8.5936534558731701</v>
+      </c>
+      <c r="N5">
+        <v>0.7440155011741032</v>
+      </c>
+      <c r="O5" s="5">
+        <f t="shared" si="0"/>
+        <v>9999.9991558131624</v>
+      </c>
+      <c r="P5" s="1">
+        <f t="shared" ref="P5:P7" si="3">K5*EXP(-E5*60*60*3)</f>
+        <v>140.02688823780028</v>
+      </c>
+      <c r="Q5" s="1">
+        <f t="shared" ref="Q5:Q7" si="4">P5*$M$10</f>
+        <v>1.1142985714411147</v>
+      </c>
+      <c r="R5">
+        <v>2.8182193194193976</v>
+      </c>
+      <c r="S5" s="5">
+        <f t="shared" ref="S5:S7" si="5">Q5*R5*3600*(1-EXP(-R5*3600*E5))</f>
+        <v>9999.9999659465193</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>84</v>
       </c>
@@ -5874,31 +6210,52 @@
         <v>10.776400000000001</v>
       </c>
       <c r="H6" s="2">
-        <v>6.4351849845382201E-3</v>
+        <f>K13*2</f>
+        <v>2.8901554404145074E-2</v>
       </c>
       <c r="I6" s="2">
         <v>2.8214400000000001E-3</v>
       </c>
       <c r="J6" s="1">
         <f>I6*$B$10*H6</f>
-        <v>182.65427252712169</v>
-      </c>
-      <c r="K6" s="1">
+        <v>820.33265667979276</v>
+      </c>
+      <c r="K6" s="26">
         <f>J6*(1-EXP(-E6*$B$12))</f>
-        <v>152.4914110262271</v>
+        <v>684.86590867684413</v>
       </c>
       <c r="L6" s="1">
-        <f>K6*EXP(-E6*60*60)</f>
-        <v>150.86541259985421</v>
+        <f t="shared" si="1"/>
+        <v>682.42298959137145</v>
       </c>
       <c r="M6" s="1">
-        <f>K6*EXP(-E6*24*60*60)</f>
-        <v>117.89859416188695</v>
-      </c>
-      <c r="O6" s="2"/>
-      <c r="Q6" s="2"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>5.4305496036507908</v>
+      </c>
+      <c r="N6">
+        <v>7.0382896477704344</v>
+      </c>
+      <c r="O6" s="5">
+        <f t="shared" si="0"/>
+        <v>9999.9999975933188</v>
+      </c>
+      <c r="P6" s="1">
+        <f t="shared" si="3"/>
+        <v>663.19074032883577</v>
+      </c>
+      <c r="Q6" s="1">
+        <f t="shared" si="4"/>
+        <v>5.27750422680539</v>
+      </c>
+      <c r="R6">
+        <v>7.1415650491012235</v>
+      </c>
+      <c r="S6" s="5">
+        <f t="shared" si="5"/>
+        <v>9999.9991257221427</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>118</v>
       </c>
@@ -5925,32 +6282,52 @@
         <v>0.42981666666666657</v>
       </c>
       <c r="H7" s="2">
-        <f>PI()*0.635^2*0.0127</f>
-        <v>1.6087962461345549E-2</v>
+        <f>K14*2</f>
+        <v>3.4993270524899062E-2</v>
       </c>
       <c r="I7" s="2">
         <v>7.2812500000000004E-4</v>
       </c>
       <c r="J7" s="1">
         <f>I7*$B$10*H7</f>
-        <v>117.84331953170232</v>
-      </c>
-      <c r="K7" s="1">
+        <v>256.32351951547781</v>
+      </c>
+      <c r="K7" s="26">
         <f>J7*(1-EXP(-E7*$B$12))</f>
-        <v>117.84331953170232</v>
+        <v>256.32351951547781</v>
       </c>
       <c r="L7" s="1">
-        <f>K7*EXP(-E7*60*60)</f>
-        <v>90.069324779102146</v>
+        <f t="shared" si="1"/>
+        <v>234.35763357931839</v>
       </c>
       <c r="M7" s="1">
-        <f>K7*EXP(-E7*24*60*60)</f>
-        <v>0.18613648633715099</v>
-      </c>
-      <c r="O7" s="2"/>
-      <c r="Q7" s="2"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>1.8649587917733839</v>
+      </c>
+      <c r="N7">
+        <v>2.8098205181566467</v>
+      </c>
+      <c r="O7" s="5">
+        <f>M7*N7*3600*(1-EXP(-N7*3600*E7))</f>
+        <v>9999.9900021951762</v>
+      </c>
+      <c r="P7" s="1">
+        <f t="shared" si="3"/>
+        <v>114.44696379926732</v>
+      </c>
+      <c r="Q7" s="1">
+        <f t="shared" si="4"/>
+        <v>0.91074000052562987</v>
+      </c>
+      <c r="R7">
+        <v>4.3985954337428037</v>
+      </c>
+      <c r="S7" s="5">
+        <f t="shared" si="5"/>
+        <v>9999.9983101279468</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="1"/>
@@ -5959,279 +6336,431 @@
       <c r="I8" s="2"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
+      <c r="L8" s="27" t="s">
+        <v>149</v>
+      </c>
       <c r="M8" s="1"/>
-      <c r="O8" s="2"/>
-      <c r="Q8" s="2"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="N8" s="1"/>
+      <c r="P8" s="2"/>
+      <c r="R8" s="2"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="O9" s="2"/>
-      <c r="Q9" s="2"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="B9" s="12"/>
+      <c r="C9" s="13"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="L9" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="M9" t="s">
+        <v>165</v>
+      </c>
+      <c r="P9" s="2"/>
+      <c r="R9" s="2"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A10" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="7">
         <f>1.006*10^7</f>
         <v>10060000</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="O10" s="2"/>
-      <c r="Q10" s="2"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="H10" s="14"/>
+      <c r="I10" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="L10" s="29">
+        <f>K4*EXP(-E4*24*60*60)</f>
+        <v>87.759164237945612</v>
+      </c>
+      <c r="M10">
+        <f>10/(4*PI()*10*10)</f>
+        <v>7.9577471545947669E-3</v>
+      </c>
+      <c r="P10" s="2"/>
+      <c r="R10" s="2"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="7">
         <v>7</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="15" t="s">
         <v>138</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
+      <c r="H11" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="I11" s="9">
+        <f>19.3</f>
+        <v>19.3</v>
+      </c>
+      <c r="J11" s="10">
+        <f>H4*I11</f>
+        <v>0.62099535100793823</v>
+      </c>
+      <c r="K11" s="10">
+        <f>J11/I11</f>
+        <v>3.2175924922691099E-2</v>
+      </c>
+      <c r="L11" s="29">
+        <f>K5*EXP(-E5*24*60*60)</f>
+        <v>1.444436214447043E-5</v>
+      </c>
       <c r="M11" s="1"/>
-      <c r="O11" s="2"/>
-      <c r="Q11" s="2"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="N11" s="1"/>
+      <c r="P11" s="2"/>
+      <c r="R11" s="2"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A12" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="7">
         <f>60*60*24*B11</f>
         <v>604800</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="15" t="s">
         <v>132</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="1"/>
+      <c r="F12" s="6">
+        <f>J13*2</f>
+        <v>0.55779999999999996</v>
+      </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
+      <c r="H12" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="I12" s="9">
+        <v>7.31</v>
+      </c>
+      <c r="J12" s="10">
+        <f>I12*H5</f>
+        <v>0.23520601118487192</v>
+      </c>
+      <c r="K12" s="10">
+        <f t="shared" ref="K12:K14" si="6">J12/I12</f>
+        <v>3.2175924922691099E-2</v>
+      </c>
+      <c r="L12" s="29">
+        <f>K6*EXP(-E6*24*60*60)</f>
+        <v>529.50344730245718</v>
+      </c>
       <c r="M12" s="1"/>
-      <c r="O12" s="2"/>
-      <c r="Q12" s="2"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="N12" s="1"/>
+      <c r="P12" s="2"/>
+      <c r="R12" s="2"/>
+    </row>
+    <row r="13" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="18" t="s">
         <v>139</v>
       </c>
+      <c r="B13" s="19"/>
+      <c r="C13" s="20"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
+      <c r="H13" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" s="9">
+        <f>19.3</f>
+        <v>19.3</v>
+      </c>
+      <c r="J13" s="10">
+        <f>0.2789</f>
+        <v>0.27889999999999998</v>
+      </c>
+      <c r="K13" s="10">
+        <f t="shared" si="6"/>
+        <v>1.4450777202072537E-2</v>
+      </c>
+      <c r="L13" s="30">
+        <f>K7*EXP(-E7*24*60*60)</f>
+        <v>0.40486944425685401</v>
+      </c>
       <c r="M13" s="1"/>
-      <c r="O13" s="2"/>
-      <c r="Q13" s="2"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N13" s="1"/>
+      <c r="P13" s="2"/>
+      <c r="R13" s="2"/>
+    </row>
+    <row r="14" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
+      <c r="H14" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="I14" s="9">
+        <f>7.43</f>
+        <v>7.43</v>
+      </c>
+      <c r="J14" s="10">
+        <f>0.13</f>
+        <v>0.13</v>
+      </c>
+      <c r="K14" s="17">
+        <f t="shared" si="6"/>
+        <v>1.7496635262449531E-2</v>
+      </c>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
-      <c r="Q14" s="2"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="N14" s="1"/>
+      <c r="R14" s="2"/>
+    </row>
+    <row r="15" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="22" t="s">
         <v>154</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
+      <c r="H15" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="J15" s="9"/>
+      <c r="K15" s="23"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
-      <c r="Q15" s="2"/>
-    </row>
-    <row r="16" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B16" s="3" t="s">
+      <c r="N15" s="1"/>
+      <c r="R15" s="2"/>
+    </row>
+    <row r="16" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="11"/>
+      <c r="B16" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="I16" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="J16" s="3" t="s">
+      <c r="J16" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="K16" s="3" t="s">
+      <c r="K16" s="25" t="s">
         <v>83</v>
       </c>
       <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="Q16" s="2"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="M16" s="1">
+        <f>Q17*2</f>
+        <v>0</v>
+      </c>
+      <c r="N16" s="1"/>
+      <c r="R16" s="2"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A17" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="7">
         <v>24</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="F17">
+      <c r="E17" s="7"/>
+      <c r="F17" s="7">
         <v>685.51</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="7">
         <v>0.33200000000000002</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="7">
         <v>479.43</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="7">
         <v>0.26600000000000001</v>
       </c>
-      <c r="Q17" s="2"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="J17" s="7"/>
+      <c r="K17" s="15"/>
+      <c r="N17" t="s">
+        <v>173</v>
+      </c>
+      <c r="R17" s="2"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="7">
         <f>54.29</f>
         <v>54.29</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="F18">
+      <c r="E18" s="7"/>
+      <c r="F18" s="7">
         <v>416.9</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="7">
         <v>0.27200000000000002</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="7">
         <v>1097.28</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="7">
         <v>0.58499999999999996</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="7">
         <v>1293.56</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="15">
         <v>0.84799999999999998</v>
       </c>
-      <c r="O18" s="2"/>
+      <c r="N18" t="s">
+        <v>176</v>
+      </c>
       <c r="P18" s="2"/>
-      <c r="R18" s="2"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="Q18" s="2"/>
+      <c r="S18" s="2"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A19" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="7">
         <f>2.6941</f>
         <v>2.6941000000000002</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="F19">
+      <c r="E19" s="7"/>
+      <c r="F19" s="7">
         <v>411.8</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="7">
         <v>0.95620000000000005</v>
       </c>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="15"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
-      <c r="P19" s="2"/>
-      <c r="R19" s="2"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="N19" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q19" s="2"/>
+      <c r="S19" s="2"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A20" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="7">
         <v>2.5789</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="F20">
+      <c r="E20" s="7"/>
+      <c r="F20" s="7">
         <v>846.8</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="7">
         <v>0.98850000000000005</v>
       </c>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="15"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="F22" t="s">
+      <c r="N20" s="1"/>
+    </row>
+    <row r="21" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="18"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="20"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="F22" s="21" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="F23" t="s">
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="21"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="F23" s="21" t="s">
         <v>157</v>
       </c>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>